<commit_message>
feat: load and interprete event mapping file
</commit_message>
<xml_diff>
--- a/moodle_default_events_list.xlsx
+++ b/moodle_default_events_list.xlsx
@@ -1109,15 +1109,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">“</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">=LEFT(</t>
+      <t xml:space="preserve">“=LEFT(</t>
     </r>
     <r>
       <rPr>
@@ -1125,6 +1117,7 @@
         <color rgb="FF0000FF"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">H9</t>
     </r>
@@ -1133,6 +1126,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">,SEARCH("\",</t>
     </r>
@@ -1142,6 +1136,7 @@
         <color rgb="FF0000FF"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">H9</t>
     </r>
@@ -1150,6 +1145,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)-2)”</t>
     </r>
@@ -1171,15 +1167,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">“</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">=RIGHT(</t>
+      <t xml:space="preserve">“=RIGHT(</t>
     </r>
     <r>
       <rPr>
@@ -1187,6 +1175,7 @@
         <color rgb="FF0000FF"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">H9</t>
     </r>
@@ -1195,6 +1184,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">,LEN(</t>
     </r>
@@ -1204,6 +1194,7 @@
         <color rgb="FF0000FF"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">H9</t>
     </r>
@@ -1212,6 +1203,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)-SEARCH("\",</t>
     </r>
@@ -1221,6 +1213,7 @@
         <color rgb="FF0000FF"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">H9</t>
     </r>
@@ -1229,6 +1222,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)+1)”</t>
     </r>
@@ -1237,25 +1231,25 @@
     <t xml:space="preserve">vague</t>
   </si>
   <si>
-    <t xml:space="preserve">Student action?</t>
+    <t xml:space="preserve">studentaction</t>
   </si>
   <si>
     <t xml:space="preserve">event name in DB</t>
   </si>
   <si>
-    <t xml:space="preserve">Novel Learning-Cycle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User-Agent-Based</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Active/Passive</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extracted Event Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Event Name</t>
+    <t xml:space="preserve">newlc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">useragentbased</t>
+  </si>
+  <si>
+    <t xml:space="preserve">activepassive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eventname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Event Name Full</t>
   </si>
   <si>
     <t xml:space="preserve">Component</t>
@@ -5493,7 +5487,7 @@
     <numFmt numFmtId="165" formatCode="General"/>
     <numFmt numFmtId="166" formatCode="0.00"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -5514,17 +5508,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -5665,7 +5648,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5781,12 +5764,12 @@
   <dimension ref="A1:N514"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="8" topLeftCell="A499" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G520" activeCellId="0" sqref="G520"/>
+      <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="7.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="41.87"/>
@@ -5878,7 +5861,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
         <v>20</v>
       </c>

</xml_diff>